<commit_message>
added updates to model
</commit_message>
<xml_diff>
--- a/USA/state/data/model_report/t2m_mean_1982_1991_DIC_values.xlsx
+++ b/USA/state/data/model_report/t2m_mean_1982_1991_DIC_values.xlsx
@@ -5,7 +5,7 @@
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/rmp15/Documents/Weekly Reports/2017/03 March 2017/March 22nd/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rmiparks/git/mortality/USA/state/data/model_report/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="13">
   <si>
     <t>sex</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>1982 - 1991</t>
+  </si>
+  <si>
+    <t>DIC average</t>
   </si>
 </sst>
 </file>
@@ -439,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="95" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="91" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -450,17 +453,17 @@
     <col min="6" max="6" width="14.83203125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F1" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F2" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -491,8 +494,14 @@
       <c r="K3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -523,8 +532,15 @@
       <c r="K4">
         <v>1705</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M4" t="s">
+        <v>4</v>
+      </c>
+      <c r="N4">
+        <f>AVERAGE(D4,D9,D14,D19,D24,J4,J9,J14,J19,J24)</f>
+        <v>33717.886999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -555,8 +571,15 @@
       <c r="K5">
         <v>2219</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N5">
+        <f>AVERAGE(D5,D10,D15,D20,D25,J5,J10,J15,J20,J25)</f>
+        <v>33726.636000000006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>1</v>
       </c>
@@ -587,8 +610,15 @@
       <c r="K6" s="6">
         <v>2384</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="N6" s="6">
+        <f t="shared" ref="N6:N8" si="0">AVERAGE(D6,D11,D16,D21,D26,J6,J11,J16,J21,J26)</f>
+        <v>33711.782000000007</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>1</v>
       </c>
@@ -619,8 +649,15 @@
       <c r="K7">
         <v>7096</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M7" t="s">
+        <v>7</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>33724.161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>1</v>
       </c>
@@ -651,8 +688,15 @@
       <c r="K8">
         <v>2632</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M8" t="s">
+        <v>8</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>33836.736000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>1</v>
       </c>
@@ -684,7 +728,7 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>1</v>
       </c>
@@ -716,7 +760,7 @@
         <v>2679</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>1</v>
       </c>
@@ -748,7 +792,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>1</v>
       </c>
@@ -780,7 +824,7 @@
         <v>6411</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>1</v>
       </c>
@@ -812,7 +856,7 @@
         <v>3083</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>1</v>
       </c>
@@ -844,7 +888,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>1</v>
       </c>
@@ -876,7 +920,7 @@
         <v>2904</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>1</v>
       </c>

</xml_diff>